<commit_message>
Task[11] v2 Detecting Emoticons.
	- Eliminate <ed> in emoticons.
	- Make regex of emoticions to satisfy detection.
	- Created a final list of emoticons.
	- Created emoticons fuzzy rules for each emotions.
</commit_message>
<xml_diff>
--- a/Gathered Emoticons.xlsx
+++ b/Gathered Emoticons.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maranan.ld\Documents\MSTR\EmoTector v2.0\EmoTector\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\Documents\CIT-U\Masters of Computer Science\Capstone - Thesis\Emotions Detection and Analysis\EmoTector\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="161">
   <si>
     <t>&lt;ed&gt;&lt;U+00A0&gt;&lt;U+00BD&gt;&lt;ed&gt;&lt;U+00B8&gt;&lt;U+0080&gt;</t>
   </si>
@@ -6421,15 +6421,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6545,13 +6545,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6909,15 +6909,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -6970,13 +6970,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
@@ -7031,13 +7031,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
@@ -7094,139 +7094,139 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="136" name="Picture 135" descr="https://www.facebook.com/images/emoji.php/v7/ff0/1/16/1f613.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2AC5A1A-5FC0-44E0-8406-6A97EC1BEE5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId105">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3857625" y="32651700"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="137" name="Picture 136" descr="https://www.facebook.com/images/emoji.php/v7/f71/1/16/1f614.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A80A14F-350E-4360-AF00-4469A4A596D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId106">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3895725" y="32918400"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="136" name="Picture 135" descr="https://www.facebook.com/images/emoji.php/v7/ff0/1/16/1f613.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2AC5A1A-5FC0-44E0-8406-6A97EC1BEE5D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId105">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3857625" y="32651700"/>
-          <a:ext cx="152400" cy="152400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="137" name="Picture 136" descr="https://www.facebook.com/images/emoji.php/v7/f71/1/16/1f614.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9A80A14F-350E-4360-AF00-4469A4A596D1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId106">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="3895725" y="32918400"/>
-          <a:ext cx="152400" cy="152400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
         <xdr:cNvPr id="138" name="Picture 137" descr="https://www.facebook.com/images/emoji.php/v7/ff2/1/16/1f615.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
@@ -7277,13 +7277,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7338,13 +7338,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7399,13 +7399,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7582,13 +7582,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7643,13 +7643,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>247650</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7704,13 +7704,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7763,15 +7763,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>219075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -7948,13 +7948,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8009,13 +8009,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>200025</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -8070,13 +8070,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>209550</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9046,13 +9046,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>257175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9107,13 +9107,13 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>228600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9227,15 +9227,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9351,13 +9351,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9410,15 +9410,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9593,15 +9593,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9654,15 +9654,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -9693,7 +9693,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5600700" y="4143375"/>
+          <a:off x="4171950" y="3038475"/>
           <a:ext cx="304800" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -10205,13 +10205,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -10262,6 +10262,62 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="152400" cy="152400"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="176" name="Picture 175" descr="https://www.facebook.com/images/emoji.php/v7/f32/1/16/1f637.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D861609-96D5-4A8E-8B4A-308EC5213FA0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId129">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="21650325" y="11944350"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -10564,8 +10620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S29" sqref="S29:T29"/>
+    <sheetView tabSelected="1" topLeftCell="W1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y2" sqref="Y2:Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21.75" customHeight="1"/>
@@ -10664,7 +10720,7 @@
         <v>99</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>123</v>
@@ -10680,14 +10736,14 @@
       <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>152</v>
+      <c r="G5" s="7" t="s">
+        <v>102</v>
       </c>
       <c r="M5" s="7" t="s">
         <v>110</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="Y5" s="6" t="s">
         <v>149</v>
@@ -10703,11 +10759,14 @@
       <c r="A6" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="G6" s="7" t="s">
+        <v>103</v>
+      </c>
       <c r="M6" s="7" t="s">
         <v>111</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="Y6" s="7" t="s">
         <v>42</v>
@@ -10723,11 +10782,14 @@
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="G7" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="M7" s="7" t="s">
         <v>135</v>
       </c>
       <c r="S7" s="7" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="Y7" s="7" t="s">
         <v>54</v>
@@ -10744,11 +10806,15 @@
         <v>6</v>
       </c>
       <c r="F8" s="1"/>
+      <c r="G8" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="L8" s="2"/>
       <c r="M8" s="4" t="s">
         <v>138</v>
       </c>
       <c r="S8" s="7" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="Y8" s="7" t="s">
         <v>122</v>
@@ -10764,11 +10830,14 @@
       <c r="A9" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="G9" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="M9" s="6" t="s">
         <v>146</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="Y9" s="7" t="s">
         <v>124</v>
@@ -10784,8 +10853,14 @@
       <c r="A10" s="7" t="s">
         <v>8</v>
       </c>
+      <c r="G10" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>138</v>
+      </c>
       <c r="S10" s="7" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="Y10" s="7" t="s">
         <v>125</v>
@@ -10801,8 +10876,11 @@
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
+      <c r="G11" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="S11" s="7" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="AF11" s="7" t="s">
         <v>41</v>
@@ -10815,8 +10893,11 @@
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="G12" s="4" t="s">
+        <v>93</v>
+      </c>
       <c r="S12" s="7" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="AF12" s="7" t="s">
         <v>43</v>
@@ -10829,8 +10910,11 @@
       <c r="A13" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="G13" s="6" t="s">
+        <v>152</v>
+      </c>
       <c r="S13" s="7" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="AF13" s="7" t="s">
         <v>44</v>
@@ -10843,8 +10927,11 @@
       <c r="A14" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="G14" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="S14" s="7" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="AF14" s="7" t="s">
         <v>45</v>
@@ -10857,8 +10944,11 @@
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
+      <c r="G15" s="7" t="s">
+        <v>129</v>
+      </c>
       <c r="S15" s="7" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="AF15" s="7" t="s">
         <v>46</v>
@@ -10873,7 +10963,7 @@
         <v>14</v>
       </c>
       <c r="S16" s="7" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="AF16" s="7" t="s">
         <v>47</v>
@@ -10887,8 +10977,8 @@
       <c r="A17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="S17" s="7" t="s">
-        <v>118</v>
+      <c r="S17" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="AF17" s="7" t="s">
         <v>48</v>
@@ -10902,8 +10992,8 @@
       <c r="A18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="S18" s="7" t="s">
-        <v>119</v>
+      <c r="S18" s="6" t="s">
+        <v>141</v>
       </c>
       <c r="AF18" s="7" t="s">
         <v>49</v>
@@ -10913,9 +11003,6 @@
       <c r="A19" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S19" s="7" t="s">
-        <v>120</v>
-      </c>
       <c r="AF19" s="7" t="s">
         <v>50</v>
       </c>
@@ -10924,10 +11011,6 @@
       <c r="A20" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="S20" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="X20" s="2"/>
       <c r="AF20" s="7" t="s">
         <v>51</v>
       </c>
@@ -10936,9 +11019,6 @@
       <c r="A21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="S21" s="7" t="s">
-        <v>136</v>
-      </c>
       <c r="AF21" s="7" t="s">
         <v>52</v>
       </c>
@@ -10946,9 +11026,6 @@
     <row r="22" spans="1:38" ht="21.75" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="S22" s="7" t="s">
-        <v>137</v>
       </c>
       <c r="AF22" s="7" t="s">
         <v>53</v>
@@ -10959,9 +11036,6 @@
       <c r="A23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S23" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="AF23" s="7" t="s">
         <v>55</v>
       </c>
@@ -10970,9 +11044,6 @@
       <c r="A24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="S24" s="4" t="s">
-        <v>95</v>
-      </c>
       <c r="AF24" s="7" t="s">
         <v>57</v>
       </c>
@@ -10980,9 +11051,6 @@
     <row r="25" spans="1:38" ht="21.75" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>141</v>
       </c>
       <c r="AF25" s="7" t="s">
         <v>59</v>
@@ -10993,9 +11061,6 @@
       <c r="A26" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="S26" s="6" t="s">
-        <v>142</v>
-      </c>
       <c r="AF26" s="7" t="s">
         <v>62</v>
       </c>
@@ -11005,9 +11070,6 @@
       <c r="A27" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="S27" s="6" t="s">
-        <v>138</v>
-      </c>
       <c r="AF27" s="7" t="s">
         <v>63</v>
       </c>
@@ -11016,9 +11078,6 @@
     <row r="28" spans="1:38" ht="21.75" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>26</v>
-      </c>
-      <c r="S28" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="AF28" s="7" t="s">
         <v>78</v>

</xml_diff>